<commit_message>
test commit verification of opening browser and report is successful
</commit_message>
<xml_diff>
--- a/demoproject/Config.xlsx
+++ b/demoproject/Config.xlsx
@@ -27,9 +27,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Browser:</t>
-  </si>
-  <si>
     <t>Chrome</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>https://www.amazon.in/</t>
+  </si>
+  <si>
+    <t>Broswer:</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,74 +438,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>